<commit_message>
preload of ephys data
</commit_message>
<xml_diff>
--- a/cook/JS_juxtacelluar_analysis/status_report_PV_JUX.xlsx
+++ b/cook/JS_juxtacelluar_analysis/status_report_PV_JUX.xlsx
@@ -219,7 +219,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF1A4E86"/>
+      <color rgb="FFF28E2B"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,7 +243,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFF28E2B"/>
+      <color rgb="FF76B7B2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -259,6 +259,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF59A14F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFE15759"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -267,7 +275,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF59A14F"/>
+      <color rgb="FFB07AA1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,15 +283,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF76B7B2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFB07AA1"/>
+      <color rgb="FF1A4E86"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>

</xml_diff>